<commit_message>
Vorläufiges Ende Reparaturnummern mit Regex suchen
</commit_message>
<xml_diff>
--- a/dst/dstFile.xlsx
+++ b/dst/dstFile.xlsx
@@ -437,7 +437,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="19" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
     <col width="50" customWidth="1" min="4" max="4"/>
@@ -448,7 +448,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Auftragsnummer</t>
+          <t>Suchergebnis</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -475,7 +475,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
@@ -493,7 +493,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
@@ -557,7 +557,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
@@ -575,7 +575,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
@@ -593,7 +593,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
@@ -611,7 +611,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
@@ -629,7 +629,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
@@ -647,7 +647,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
@@ -670,7 +670,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
@@ -693,7 +693,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
@@ -762,7 +762,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
@@ -849,7 +849,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
@@ -890,7 +890,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
@@ -913,7 +913,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
@@ -931,7 +931,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
@@ -954,7 +954,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
@@ -1018,7 +1018,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
@@ -1036,7 +1036,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
@@ -1123,7 +1123,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
@@ -1169,7 +1169,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
@@ -1233,7 +1233,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
@@ -1256,7 +1256,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
@@ -1279,7 +1279,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 107-13068</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
@@ -1302,7 +1302,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B41" s="2" t="n">
@@ -1320,7 +1320,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B42" s="2" t="n">
@@ -1338,7 +1338,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B43" s="2" t="n">
@@ -1356,7 +1356,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B44" s="2" t="n">
@@ -1379,7 +1379,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B45" s="2" t="n">
@@ -1397,7 +1397,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B46" s="2" t="n">
@@ -1420,7 +1420,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B47" s="2" t="n">
@@ -1438,7 +1438,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B48" s="2" t="n">
@@ -1461,7 +1461,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B49" s="2" t="n">
@@ -1484,7 +1484,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B50" s="2" t="n">
@@ -1502,7 +1502,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>m200-222448</t>
+          <t>M200-222448</t>
         </is>
       </c>
       <c r="B51" s="2" t="n">
@@ -1525,7 +1525,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B52" s="2" t="n">
@@ -1543,7 +1543,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B53" s="2" t="n">
@@ -1612,7 +1612,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B56" s="2" t="n">
@@ -1676,7 +1676,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B59" s="2" t="n">
@@ -1717,7 +1717,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B61" s="2" t="n">
@@ -1740,7 +1740,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B62" s="2" t="n">
@@ -1781,7 +1781,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B64" s="2" t="n">
@@ -1827,7 +1827,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B66" s="2" t="n">
@@ -1891,7 +1891,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B69" s="2" t="n">
@@ -1955,7 +1955,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B72" s="2" t="n">
@@ -1973,7 +1973,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B73" s="2" t="n">
@@ -1996,7 +1996,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B74" s="2" t="n">
@@ -2014,7 +2014,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B75" s="2" t="n">
@@ -2037,7 +2037,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B76" s="2" t="n">
@@ -2060,7 +2060,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B77" s="2" t="n">
@@ -2083,7 +2083,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B78" s="2" t="n">
@@ -2101,7 +2101,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B79" s="2" t="n">
@@ -2119,7 +2119,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B80" s="2" t="n">
@@ -2137,7 +2137,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B81" s="2" t="n">
@@ -2155,7 +2155,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B82" s="2" t="n">
@@ -2173,7 +2173,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B83" s="2" t="n">
@@ -2191,7 +2191,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B84" s="2" t="n">
@@ -2232,7 +2232,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B86" s="2" t="n">
@@ -2250,7 +2250,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B87" s="2" t="n">
@@ -2314,7 +2314,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B90" s="2" t="n">
@@ -2332,7 +2332,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B91" s="2" t="n">
@@ -2350,7 +2350,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B92" s="2" t="n">
@@ -2368,7 +2368,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B93" s="2" t="n">
@@ -2391,7 +2391,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B94" s="2" t="n">
@@ -2409,7 +2409,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B95" s="2" t="n">
@@ -2427,7 +2427,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>M043-17470</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B96" s="2" t="n">
@@ -2450,7 +2450,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B97" s="2" t="n">
@@ -2468,7 +2468,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B98" s="2" t="n">
@@ -2514,7 +2514,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B100" s="2" t="n">
@@ -2532,7 +2532,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B101" s="2" t="n">
@@ -2550,7 +2550,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B102" s="2" t="n">
@@ -2568,7 +2568,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B103" s="2" t="n">
@@ -2591,7 +2591,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B104" s="2" t="n">
@@ -2660,7 +2660,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B107" s="2" t="n">
@@ -2678,7 +2678,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B108" s="2" t="n">
@@ -2696,7 +2696,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B109" s="2" t="n">
@@ -2714,7 +2714,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B110" s="2" t="n">
@@ -2732,7 +2732,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B111" s="2" t="n">
@@ -2755,7 +2755,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B112" s="2" t="n">
@@ -2773,7 +2773,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B113" s="2" t="n">
@@ -2791,7 +2791,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B114" s="2" t="n">
@@ -2809,7 +2809,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B115" s="2" t="n">
@@ -2850,7 +2850,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B117" s="2" t="n">
@@ -2868,7 +2868,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B118" s="2" t="n">
@@ -2886,7 +2886,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B119" s="2" t="n">
@@ -2927,7 +2927,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>s021-12695</t>
+          <t>S021-12695</t>
         </is>
       </c>
       <c r="B121" s="2" t="n">
@@ -2950,7 +2950,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B122" s="2" t="n">
@@ -3019,7 +3019,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B125" s="2" t="n">
@@ -3037,7 +3037,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B126" s="2" t="n">
@@ -3055,7 +3055,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B127" s="2" t="n">
@@ -3119,7 +3119,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B130" s="2" t="n">
@@ -3160,7 +3160,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B132" s="2" t="n">
@@ -3178,7 +3178,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B133" s="2" t="n">
@@ -3196,7 +3196,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B134" s="2" t="n">
@@ -3237,7 +3237,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B136" s="2" t="n">
@@ -3255,7 +3255,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B137" s="2" t="n">
@@ -3273,7 +3273,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B138" s="2" t="n">
@@ -3360,7 +3360,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B142" s="2" t="n">
@@ -3378,7 +3378,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B143" s="2" t="n">
@@ -3396,7 +3396,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B144" s="2" t="n">
@@ -3414,7 +3414,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B145" s="2" t="n">
@@ -3432,7 +3432,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B146" s="2" t="n">
@@ -3450,7 +3450,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B147" s="2" t="n">
@@ -3468,7 +3468,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B148" s="2" t="n">
@@ -3486,7 +3486,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B149" s="2" t="n">
@@ -3504,7 +3504,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B150" s="2" t="n">
@@ -3527,7 +3527,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B151" s="2" t="n">
@@ -3568,7 +3568,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B153" s="2" t="n">
@@ -3586,7 +3586,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B154" s="2" t="n">
@@ -3604,7 +3604,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B155" s="2" t="n">
@@ -3622,7 +3622,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B156" s="2" t="n">
@@ -3640,7 +3640,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B157" s="2" t="n">
@@ -3658,7 +3658,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B158" s="2" t="n">
@@ -3681,7 +3681,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B159" s="2" t="n">
@@ -3699,7 +3699,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B160" s="2" t="n">
@@ -3717,7 +3717,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B161" s="2" t="n">
@@ -3735,7 +3735,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B162" s="2" t="n">
@@ -3753,7 +3753,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B163" s="2" t="n">
@@ -3771,7 +3771,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>1_Nichts gefunden</t>
+          <t>1_Keine Reparaturnummer gefunden</t>
         </is>
       </c>
       <c r="B164" s="2" t="n">
@@ -3794,7 +3794,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B165" s="2" t="n">
@@ -3812,7 +3812,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B166" s="2" t="n">
@@ -3830,7 +3830,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>1_Suchfeld ist leer</t>
+          <t>1_Das zu durchsuchende Feld ist leer</t>
         </is>
       </c>
       <c r="B167" s="2" t="n">

</xml_diff>